<commit_message>
Ver-2.1.1 1. `num_of_components` metric has been added. 2. Results have been renewed.
</commit_message>
<xml_diff>
--- a/result/Database_indiv.xlsx
+++ b/result/Database_indiv.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>level_of_deepest_hierarchy</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>num_of_components</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -518,6 +523,9 @@
       <c r="J2" t="n">
         <v>4</v>
       </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -552,6 +560,9 @@
       <c r="J3" t="n">
         <v>3</v>
       </c>
+      <c r="K3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -586,6 +597,9 @@
       <c r="J4" t="n">
         <v>1</v>
       </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -620,6 +634,9 @@
       <c r="J5" t="n">
         <v>1</v>
       </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -654,6 +671,9 @@
       <c r="J6" t="n">
         <v>2</v>
       </c>
+      <c r="K6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -688,6 +708,9 @@
       <c r="J7" t="n">
         <v>3</v>
       </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -722,6 +745,9 @@
       <c r="J8" t="n">
         <v>3</v>
       </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -756,6 +782,9 @@
       <c r="J9" t="n">
         <v>4</v>
       </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -790,6 +819,9 @@
       <c r="J10" t="n">
         <v>1</v>
       </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -824,6 +856,9 @@
       <c r="J11" t="n">
         <v>1</v>
       </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -858,6 +893,9 @@
       <c r="J12" t="n">
         <v>4</v>
       </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -892,6 +930,9 @@
       <c r="J13" t="n">
         <v>6</v>
       </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -926,6 +967,9 @@
       <c r="J14" t="n">
         <v>5</v>
       </c>
+      <c r="K14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -960,6 +1004,9 @@
       <c r="J15" t="n">
         <v>1</v>
       </c>
+      <c r="K15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -994,6 +1041,9 @@
       <c r="J16" t="n">
         <v>5</v>
       </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1028,6 +1078,9 @@
       <c r="J17" t="n">
         <v>6</v>
       </c>
+      <c r="K17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1062,6 +1115,9 @@
       <c r="J18" t="n">
         <v>2</v>
       </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1096,6 +1152,9 @@
       <c r="J19" t="n">
         <v>6</v>
       </c>
+      <c r="K19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1130,6 +1189,9 @@
       <c r="J20" t="n">
         <v>5</v>
       </c>
+      <c r="K20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1164,6 +1226,9 @@
       <c r="J21" t="n">
         <v>1</v>
       </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1198,6 +1263,9 @@
       <c r="J22" t="n">
         <v>1</v>
       </c>
+      <c r="K22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1232,6 +1300,9 @@
       <c r="J23" t="n">
         <v>5</v>
       </c>
+      <c r="K23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1266,6 +1337,9 @@
       <c r="J24" t="n">
         <v>5</v>
       </c>
+      <c r="K24" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -1300,6 +1374,9 @@
       <c r="J25" t="n">
         <v>1</v>
       </c>
+      <c r="K25" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1334,6 +1411,9 @@
       <c r="J26" t="n">
         <v>6</v>
       </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -1368,6 +1448,9 @@
       <c r="J27" t="n">
         <v>6</v>
       </c>
+      <c r="K27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -1402,6 +1485,9 @@
       <c r="J28" t="n">
         <v>4</v>
       </c>
+      <c r="K28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -1436,6 +1522,9 @@
       <c r="J29" t="n">
         <v>1</v>
       </c>
+      <c r="K29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -1470,6 +1559,9 @@
       <c r="J30" t="n">
         <v>1</v>
       </c>
+      <c r="K30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -1504,6 +1596,9 @@
       <c r="J31" t="n">
         <v>1</v>
       </c>
+      <c r="K31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -1538,6 +1633,9 @@
       <c r="J32" t="n">
         <v>6</v>
       </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -1572,6 +1670,9 @@
       <c r="J33" t="n">
         <v>1</v>
       </c>
+      <c r="K33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -1606,6 +1707,9 @@
       <c r="J34" t="n">
         <v>5</v>
       </c>
+      <c r="K34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -1640,6 +1744,9 @@
       <c r="J35" t="n">
         <v>3</v>
       </c>
+      <c r="K35" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -1674,6 +1781,9 @@
       <c r="J36" t="n">
         <v>1</v>
       </c>
+      <c r="K36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -1708,6 +1818,9 @@
       <c r="J37" t="n">
         <v>3</v>
       </c>
+      <c r="K37" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -1742,6 +1855,9 @@
       <c r="J38" t="n">
         <v>5</v>
       </c>
+      <c r="K38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -1776,6 +1892,9 @@
       <c r="J39" t="n">
         <v>6</v>
       </c>
+      <c r="K39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -1810,6 +1929,9 @@
       <c r="J40" t="n">
         <v>1</v>
       </c>
+      <c r="K40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -1844,6 +1966,9 @@
       <c r="J41" t="n">
         <v>7</v>
       </c>
+      <c r="K41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -1878,6 +2003,9 @@
       <c r="J42" t="n">
         <v>1</v>
       </c>
+      <c r="K42" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -1912,6 +2040,9 @@
       <c r="J43" t="n">
         <v>3</v>
       </c>
+      <c r="K43" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -1946,6 +2077,9 @@
       <c r="J44" t="n">
         <v>4</v>
       </c>
+      <c r="K44" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -1980,6 +2114,9 @@
       <c r="J45" t="n">
         <v>6</v>
       </c>
+      <c r="K45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -2014,6 +2151,9 @@
       <c r="J46" t="n">
         <v>3</v>
       </c>
+      <c r="K46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -2048,6 +2188,9 @@
       <c r="J47" t="n">
         <v>1</v>
       </c>
+      <c r="K47" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -2082,6 +2225,9 @@
       <c r="J48" t="n">
         <v>5</v>
       </c>
+      <c r="K48" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -2116,6 +2262,9 @@
       <c r="J49" t="n">
         <v>3</v>
       </c>
+      <c r="K49" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -2150,6 +2299,9 @@
       <c r="J50" t="n">
         <v>6</v>
       </c>
+      <c r="K50" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -2184,6 +2336,9 @@
       <c r="J51" t="n">
         <v>5</v>
       </c>
+      <c r="K51" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -2218,6 +2373,9 @@
       <c r="J52" t="n">
         <v>4</v>
       </c>
+      <c r="K52" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -2252,6 +2410,9 @@
       <c r="J53" t="n">
         <v>1</v>
       </c>
+      <c r="K53" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -2286,6 +2447,9 @@
       <c r="J54" t="n">
         <v>5</v>
       </c>
+      <c r="K54" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -2320,6 +2484,9 @@
       <c r="J55" t="n">
         <v>1</v>
       </c>
+      <c r="K55" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -2354,6 +2521,9 @@
       <c r="J56" t="n">
         <v>4</v>
       </c>
+      <c r="K56" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -2388,6 +2558,9 @@
       <c r="J57" t="n">
         <v>3</v>
       </c>
+      <c r="K57" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -2422,6 +2595,9 @@
       <c r="J58" t="n">
         <v>6</v>
       </c>
+      <c r="K58" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -2456,6 +2632,9 @@
       <c r="J59" t="n">
         <v>6</v>
       </c>
+      <c r="K59" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -2490,6 +2669,9 @@
       <c r="J60" t="n">
         <v>3</v>
       </c>
+      <c r="K60" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -2524,6 +2706,9 @@
       <c r="J61" t="n">
         <v>4</v>
       </c>
+      <c r="K61" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -2558,6 +2743,9 @@
       <c r="J62" t="n">
         <v>7</v>
       </c>
+      <c r="K62" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -2592,6 +2780,9 @@
       <c r="J63" t="n">
         <v>6</v>
       </c>
+      <c r="K63" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -2626,6 +2817,9 @@
       <c r="J64" t="n">
         <v>1</v>
       </c>
+      <c r="K64" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -2660,6 +2854,9 @@
       <c r="J65" t="n">
         <v>6</v>
       </c>
+      <c r="K65" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -2694,6 +2891,9 @@
       <c r="J66" t="n">
         <v>5</v>
       </c>
+      <c r="K66" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -2728,6 +2928,9 @@
       <c r="J67" t="n">
         <v>4</v>
       </c>
+      <c r="K67" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -2762,6 +2965,9 @@
       <c r="J68" t="n">
         <v>4</v>
       </c>
+      <c r="K68" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -2796,6 +3002,9 @@
       <c r="J69" t="n">
         <v>1</v>
       </c>
+      <c r="K69" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -2830,6 +3039,9 @@
       <c r="J70" t="n">
         <v>6</v>
       </c>
+      <c r="K70" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -2864,6 +3076,9 @@
       <c r="J71" t="n">
         <v>4</v>
       </c>
+      <c r="K71" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -2898,6 +3113,9 @@
       <c r="J72" t="n">
         <v>5</v>
       </c>
+      <c r="K72" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -2932,6 +3150,9 @@
       <c r="J73" t="n">
         <v>4</v>
       </c>
+      <c r="K73" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -2966,6 +3187,9 @@
       <c r="J74" t="n">
         <v>6</v>
       </c>
+      <c r="K74" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
@@ -3000,6 +3224,9 @@
       <c r="J75" t="n">
         <v>1</v>
       </c>
+      <c r="K75" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -3034,6 +3261,9 @@
       <c r="J76" t="n">
         <v>5</v>
       </c>
+      <c r="K76" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -3068,6 +3298,9 @@
       <c r="J77" t="n">
         <v>1</v>
       </c>
+      <c r="K77" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -3102,6 +3335,9 @@
       <c r="J78" t="n">
         <v>1</v>
       </c>
+      <c r="K78" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -3136,6 +3372,9 @@
       <c r="J79" t="n">
         <v>4</v>
       </c>
+      <c r="K79" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
@@ -3170,6 +3409,9 @@
       <c r="J80" t="n">
         <v>1</v>
       </c>
+      <c r="K80" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
@@ -3204,6 +3446,9 @@
       <c r="J81" t="n">
         <v>1</v>
       </c>
+      <c r="K81" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -3238,6 +3483,9 @@
       <c r="J82" t="n">
         <v>1</v>
       </c>
+      <c r="K82" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
@@ -3272,6 +3520,9 @@
       <c r="J83" t="n">
         <v>6</v>
       </c>
+      <c r="K83" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
@@ -3306,6 +3557,9 @@
       <c r="J84" t="n">
         <v>5</v>
       </c>
+      <c r="K84" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
@@ -3340,6 +3594,9 @@
       <c r="J85" t="n">
         <v>4</v>
       </c>
+      <c r="K85" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
@@ -3374,6 +3631,9 @@
       <c r="J86" t="n">
         <v>6</v>
       </c>
+      <c r="K86" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
@@ -3408,6 +3668,9 @@
       <c r="J87" t="n">
         <v>1</v>
       </c>
+      <c r="K87" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
@@ -3442,6 +3705,9 @@
       <c r="J88" t="n">
         <v>4</v>
       </c>
+      <c r="K88" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
@@ -3476,6 +3742,9 @@
       <c r="J89" t="n">
         <v>1</v>
       </c>
+      <c r="K89" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
@@ -3510,6 +3779,9 @@
       <c r="J90" t="n">
         <v>1</v>
       </c>
+      <c r="K90" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
@@ -3544,6 +3816,9 @@
       <c r="J91" t="n">
         <v>5</v>
       </c>
+      <c r="K91" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
@@ -3578,6 +3853,9 @@
       <c r="J92" t="n">
         <v>1</v>
       </c>
+      <c r="K92" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
@@ -3611,6 +3889,9 @@
       </c>
       <c r="J93" t="n">
         <v>8</v>
+      </c>
+      <c r="K93" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>